<commit_message>
work on D-560-3/9 and similar added to cons and params table
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.xlsx
+++ b/docs/Manual/source/tab/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="TGZ-D-48-13_26" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,16 +28,18 @@
     <sheet name="TGZ-S-400-10_20" sheetId="18" state="visible" r:id="rId20"/>
     <sheet name="TGZ-S-400-14_30" sheetId="19" state="visible" r:id="rId21"/>
     <sheet name="TGZ-D-560-3_9" sheetId="20" state="visible" r:id="rId22"/>
-    <sheet name="TGZ-D-560-30_50" sheetId="21" state="visible" r:id="rId23"/>
-    <sheet name="TGS-320-10_15" sheetId="22" state="visible" r:id="rId24"/>
-    <sheet name="TGS-560-25_50" sheetId="23" state="visible" r:id="rId25"/>
-    <sheet name="TGS-560-50_100" sheetId="24" state="visible" r:id="rId26"/>
-    <sheet name="TGMmini" sheetId="25" state="visible" r:id="rId27"/>
-    <sheet name="TGMcontroller" sheetId="26" state="visible" r:id="rId28"/>
-    <sheet name="TGZpMotion" sheetId="27" state="visible" r:id="rId29"/>
-    <sheet name="commonHW_DI" sheetId="28" state="visible" r:id="rId30"/>
-    <sheet name="commonHW_DO" sheetId="29" state="visible" r:id="rId31"/>
-    <sheet name="commonHW_AI" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="TGZ-D-560-7_15" sheetId="21" state="visible" r:id="rId23"/>
+    <sheet name="TGZ-D-560-10_20" sheetId="22" state="visible" r:id="rId24"/>
+    <sheet name="TGZ-D-560-30_50" sheetId="23" state="visible" r:id="rId25"/>
+    <sheet name="TGS-320-10_15" sheetId="24" state="visible" r:id="rId26"/>
+    <sheet name="TGS-560-25_50" sheetId="25" state="visible" r:id="rId27"/>
+    <sheet name="TGS-560-50_100" sheetId="26" state="visible" r:id="rId28"/>
+    <sheet name="TGMmini" sheetId="27" state="visible" r:id="rId29"/>
+    <sheet name="TGMcontroller" sheetId="28" state="visible" r:id="rId30"/>
+    <sheet name="TGZpMotion" sheetId="29" state="visible" r:id="rId31"/>
+    <sheet name="commonHW_DI" sheetId="30" state="visible" r:id="rId32"/>
+    <sheet name="commonHW_DO" sheetId="31" state="visible" r:id="rId33"/>
+    <sheet name="commonHW_AI" sheetId="32" state="visible" r:id="rId34"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="291">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -4006,7 +4008,7 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4248,6 +4250,488 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4481,7 +4965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4689,7 +5173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4905,7 +5389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5145,7 +5629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5328,7 +5812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5513,7 +5997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -5661,721 +6145,6 @@
       </c>
       <c r="B17" s="1" t="s">
         <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="26.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.24"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="J9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="26.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.24"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G5" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>300</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6614,6 +6383,721 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="26.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="30.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
TGZ/TGZ-D-560-x/y new description images, new parameters
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/parameters.xlsx
+++ b/docs/Manual/source/tab/parameters.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="301">
   <si>
     <t xml:space="preserve">NAPÁJENÍ</t>
   </si>
@@ -515,10 +515,64 @@
     <t xml:space="preserve">24 VDC ± 10 %, 2 A*</t>
   </si>
   <si>
+    <t xml:space="preserve">140-600 VDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,4 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 9 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSTUPY/VÝSTUPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 3pin WEIDMÜLLER BLZ 7.62HP/03/180LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 5pin WEIDMÜLLER BCZ 3.81/05/180F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 6pin WEIDMÜLLER  BLZ 7.62HP/06/180LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 8pin WEIDMÜLLER B2CF 3.50/08/180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 x 12pin WEIDMÜLLER B2CF 3.50/12/180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtr obsahující napájecí modul TGS-560-25/50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,8 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x 20 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 W</t>
+  </si>
+  <si>
     <t xml:space="preserve">24-560 VDC</t>
   </si>
   <si>
-    <t xml:space="preserve">10kW</t>
+    <t xml:space="preserve">33 kW</t>
   </si>
   <si>
     <t xml:space="preserve">60 A</t>
@@ -527,9 +581,6 @@
     <t xml:space="preserve">900 W</t>
   </si>
   <si>
-    <t xml:space="preserve">VSTUPY/VÝSTUPY</t>
-  </si>
-  <si>
     <t xml:space="preserve">šroubovací svorky M8x12</t>
   </si>
   <si>
@@ -539,18 +590,9 @@
     <t xml:space="preserve">2 x 4pin  WEIDMÜLLER LSF</t>
   </si>
   <si>
-    <t xml:space="preserve">2 x 8pin WEIDMÜLLER B2CF 3.50/08/180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 x 12pin WEIDMÜLLER B2CF 3.50/12/180</t>
-  </si>
-  <si>
     <t xml:space="preserve">Filtr obsahující napájecí modul TGS-560</t>
   </si>
   <si>
-    <t xml:space="preserve">33 kW</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vstupní napětí (VAC - 50/60 Hz) </t>
   </si>
   <si>
@@ -560,9 +602,6 @@
     <t xml:space="preserve">Maximální vstupní proud (AC) </t>
   </si>
   <si>
-    <t xml:space="preserve">16 A</t>
-  </si>
-  <si>
     <t xml:space="preserve">Výstupní napětí (DC) </t>
   </si>
   <si>
@@ -659,19 +698,10 @@
     <t xml:space="preserve">400 W</t>
   </si>
   <si>
-    <t xml:space="preserve">100 W</t>
-  </si>
-  <si>
     <t xml:space="preserve">32 A</t>
   </si>
   <si>
-    <t xml:space="preserve">1 x 5pin WEIDMÜLLER BCZ 3.81/05/180F</t>
-  </si>
-  <si>
     <t xml:space="preserve">3 x 400 VAC/50Hz 63A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150 W</t>
   </si>
   <si>
     <t xml:space="preserve">63 A</t>
@@ -2765,7 +2795,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3273,7 +3303,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4006,229 +4036,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>150</v>
+      <c r="B5" s="0" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="0" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
+      <c r="B7" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>157</v>
+      <c r="B8" s="0" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="0" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>159</v>
+      <c r="B24" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>160</v>
+      <c r="B25" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
+      <c r="B26" s="0" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>161</v>
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A28" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>163</v>
+      <c r="B28" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A31" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>164</v>
+      <c r="B31" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4247,229 +4269,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>155</v>
+      <c r="B4" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>150</v>
+      <c r="B5" s="0" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>156</v>
+      <c r="B6" s="0" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
+      <c r="B7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>157</v>
+      <c r="B8" s="0" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="0" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>159</v>
+      <c r="B24" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>160</v>
+      <c r="B25" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
+      <c r="B26" s="0" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>161</v>
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A28" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>163</v>
+      <c r="B28" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A31" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>164</v>
+      <c r="B31" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4488,229 +4502,221 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>155</v>
+      <c r="B4" s="0" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>150</v>
+      <c r="B5" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>156</v>
+      <c r="B6" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
+      <c r="B7" s="0" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>157</v>
+      <c r="B8" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="0" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>159</v>
+      <c r="B24" s="0" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>160</v>
+      <c r="B25" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
+      <c r="B26" s="0" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>161</v>
+      <c r="A27" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A28" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>163</v>
+      <c r="B28" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A31" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>164</v>
+      <c r="B31" s="0" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4762,7 +4768,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4770,7 +4776,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +4792,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4802,7 +4808,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4847,7 +4853,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -4898,7 +4904,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +4912,7 @@
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4922,7 +4928,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +4936,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4938,7 +4944,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,7 +4957,7 @@
         <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -4993,16 +4999,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>169</v>
@@ -5011,73 +5017,73 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5092,7 +5098,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -5100,18 +5106,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5127,12 +5133,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -5140,7 +5146,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>128</v>
@@ -5148,18 +5154,18 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5201,16 +5207,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -5219,25 +5225,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -5246,25 +5252,25 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -5273,19 +5279,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -5300,7 +5306,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -5308,18 +5314,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5335,12 +5341,12 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -5351,12 +5357,12 @@
         <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
@@ -5364,7 +5370,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
@@ -5372,10 +5378,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -5425,16 +5431,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -5443,16 +5449,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -5461,7 +5467,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>56</v>
@@ -5470,25 +5476,25 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -5497,19 +5503,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5524,7 +5530,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5532,18 +5538,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5559,12 +5565,12 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -5575,47 +5581,47 @@
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -5657,28 +5663,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5696,19 +5702,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -5723,28 +5729,28 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -5762,16 +5768,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -5779,10 +5785,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5790,15 +5796,15 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5840,28 +5846,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -5906,10 +5912,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -5927,10 +5933,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -5939,7 +5945,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -5948,7 +5954,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>37</v>
@@ -5959,7 +5965,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6025,28 +6031,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -6091,10 +6097,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C10" s="3"/>
     </row>
@@ -6112,10 +6118,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -6124,7 +6130,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -6136,7 +6142,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,107 +6410,107 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6512,16 +6518,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>2.05</v>
@@ -6547,16 +6553,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>2.05</v>
@@ -6582,16 +6588,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2.05</v>
@@ -6617,16 +6623,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2.05</v>
@@ -6652,16 +6658,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.05</v>
@@ -6687,16 +6693,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.05</v>
@@ -6722,16 +6728,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1.25</v>
@@ -6757,16 +6763,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.25</v>
@@ -6823,89 +6829,89 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6925,7 +6931,7 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>300</v>
@@ -6954,7 +6960,7 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>300</v>
@@ -6983,7 +6989,7 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>300</v>
@@ -7012,7 +7018,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>300</v>
@@ -7041,7 +7047,7 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>300</v>
@@ -7070,7 +7076,7 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>300</v>
@@ -7114,44 +7120,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7159,7 +7165,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
@@ -7173,7 +7179,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>11</v>

</xml_diff>